<commit_message>
working code with yml
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/executor_smoke.xlsx
+++ b/src/test/resources/testData/executor_smoke.xlsx
@@ -3,14 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adithiya Baskaran\eclipse-workspace\seleniumJavaTestNg\src\test\resources\testData\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{156467A8-97EB-4263-A641-1CE36DAAAC30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{08C1766E-951E-48D7-8EE8-0B94C36FC12B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="29070" windowHeight="16500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Testcases" sheetId="1" r:id="rId1"/>
@@ -18,6 +13,7 @@
     <sheet name="GlobalParams" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1:Q19"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -491,8 +487,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -583,8 +579,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB224328-A503-4EFB-8961-DDA5EF572FBF}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -741,7 +737,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>